<commit_message>
Added IP checksum routine
</commit_message>
<xml_diff>
--- a/EthernetFrame.xlsx
+++ b/EthernetFrame.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Ethernet frame</t>
   </si>
@@ -111,13 +111,31 @@
   </si>
   <si>
     <t>Checksum</t>
+  </si>
+  <si>
+    <t>offset (hex)</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Length (as below)</t>
+  </si>
+  <si>
+    <t>Pseudo header for checksum only</t>
+  </si>
+  <si>
+    <t>Zero byte</t>
+  </si>
+  <si>
+    <t>"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +145,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -154,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -162,6 +188,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,320 +506,525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="10.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="str">
+        <f>DEC2HEX(A4,2)</f>
+        <v>00</v>
+      </c>
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>B4+A4</f>
+        <f>C4+A4</f>
         <v>6</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="str">
+        <f t="shared" ref="B5:B40" si="0">DEC2HEX(A5,2)</f>
+        <v>06</v>
+      </c>
+      <c r="C5" s="1">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f>B5+A5</f>
+        <f>C5+A5</f>
         <v>12</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0C</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>14</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0E</v>
+      </c>
+      <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f>A10+B10</f>
+        <f>A10+C10</f>
         <v>15</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0F</v>
+      </c>
+      <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f>A11+B11</f>
+        <f>A11+C11</f>
         <v>16</v>
       </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" ref="A13:A20" si="0">A12+B12</f>
+        <f t="shared" ref="A13:A19" si="1">A12+C12</f>
         <v>18</v>
       </c>
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B17" s="1">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="C18" s="1">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1E</v>
+      </c>
+      <c r="C19" s="1">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>14</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0E</v>
+      </c>
+      <c r="C23" s="1">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>A23+B23</f>
+        <f>A23+C23</f>
         <v>20</v>
       </c>
-      <c r="B24" s="1">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f>A24+B24</f>
+        <f>A24+C24</f>
         <v>22</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C25" s="1">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" ref="A26:A28" si="1">A25+B25</f>
+        <f t="shared" ref="A26:A28" si="2">A25+C25</f>
         <v>28</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1C</v>
+      </c>
+      <c r="C26" s="1">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="1">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="1">
         <v>4</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f t="shared" ref="A31:A34" si="3">A32-C31</f>
+        <v>22</v>
+      </c>
+      <c r="B31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C31" s="3">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="B32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="C32" s="3">
+        <v>4</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="1">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>1E</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>1F</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <f>A36-C35</f>
+        <v>32</v>
+      </c>
+      <c r="B35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f>A32+B32</f>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f>A36+C36</f>
         <v>36</v>
       </c>
-      <c r="B33" s="1">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <f t="shared" ref="A34:A35" si="2">A33+B33</f>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f t="shared" ref="A38:A39" si="4">A37+C37</f>
         <v>38</v>
       </c>
-      <c r="B34" s="1">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <f t="shared" si="2"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="B35" s="1">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>28</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f>A39+C39</f>
+        <v>42</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2A</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further development and code refactoring
</commit_message>
<xml_diff>
--- a/EthernetFrame.xlsx
+++ b/EthernetFrame.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Ethernet frame</t>
   </si>
@@ -86,12 +86,6 @@
     <t>Hardware and protocol</t>
   </si>
   <si>
-    <t>Senders MAC</t>
-  </si>
-  <si>
-    <t>Senders IP</t>
-  </si>
-  <si>
     <t>Target MAC</t>
   </si>
   <si>
@@ -129,6 +123,15 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>Sender's MAC</t>
+  </si>
+  <si>
+    <t>Sender's IP</t>
+  </si>
+  <si>
+    <t>Total length</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -636,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -800,7 +803,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,7 +819,7 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -832,7 +835,7 @@
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -848,12 +851,12 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,7 +875,7 @@
         <v>16</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -891,7 +894,7 @@
         <v>17</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -907,10 +910,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -929,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,10 +948,10 @@
         <v>2</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -979,7 +982,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,7 +1027,7 @@
         <v>2A</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>